<commit_message>
complete framework UI API database
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Batch14Excel.xlsx
+++ b/src/test/resources/testdata/Batch14Excel.xlsx
@@ -37,40 +37,40 @@
     <t>confirmPassword</t>
   </si>
   <si>
-    <t>Ramzi</t>
+    <t>Yassin</t>
   </si>
   <si>
     <t>ms</t>
   </si>
   <si>
-    <t>Takada</t>
+    <t>Boufal45</t>
   </si>
   <si>
     <t>C:\Users\Abdel\OneDrive\Desktop\cat.jpg</t>
   </si>
   <si>
-    <t>Ramzi123</t>
+    <t>HakimiBest15</t>
   </si>
   <si>
     <t>Syntax123!</t>
   </si>
   <si>
-    <t>MohaHassan</t>
-  </si>
-  <si>
-    <t>Adouar</t>
-  </si>
-  <si>
-    <t>Adouar456</t>
-  </si>
-  <si>
-    <t>Lfkih</t>
-  </si>
-  <si>
-    <t>Akram</t>
-  </si>
-  <si>
-    <t>Akram789</t>
+    <t>Lahcen13</t>
+  </si>
+  <si>
+    <t>Lamar</t>
+  </si>
+  <si>
+    <t>Lamar30</t>
+  </si>
+  <si>
+    <t>AssadAllah</t>
+  </si>
+  <si>
+    <t>Demaria</t>
+  </si>
+  <si>
+    <t>AssadAllh</t>
   </si>
 </sst>
 </file>
@@ -79,9 +79,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -92,6 +92,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -101,12 +123,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -118,6 +141,14 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -145,21 +176,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -176,11 +192,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -193,44 +223,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -245,13 +245,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,169 +395,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,6 +436,17 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -488,6 +499,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -502,21 +528,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -525,23 +536,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -559,130 +559,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1012,14 +1012,14 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="12.4444444444444" customWidth="1"/>
     <col min="2" max="2" width="12.2222222222222" customWidth="1"/>
-    <col min="3" max="3" width="11.5555555555556" customWidth="1"/>
+    <col min="3" max="3" width="16.2222222222222" customWidth="1"/>
     <col min="4" max="4" width="36.3240740740741" customWidth="1"/>
     <col min="5" max="5" width="14.7777777777778" customWidth="1"/>
     <col min="6" max="6" width="10.7777777777778" customWidth="1"/>

</xml_diff>